<commit_message>
Updated con terra Spain Accelerator to 2024
</commit_message>
<xml_diff>
--- a/Resources/AcceleratorES/Data/CortesTrafico.xlsx
+++ b/Resources/AcceleratorES/Data/CortesTrafico.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conterrade-my.sharepoint.com/personal/f_gordo_conterra_es/Documents/Dokumente/3.FME Accelerator/FME Data/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conterrade-my.sharepoint.com/personal/i_costas_conterra_es/Documents/07_Schulungs/FMEAccelerator/Datos_ct/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_53451BBFC999197F00C3F4A5E8012D1611047BAC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E45F7394-E0FF-42DC-9996-9789F8539A61}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_E215B11F661493B5CBCBA328300A80A6BFFB87C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC9735DF-F1BA-4606-8ACE-56194FA0BBCC}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3816" yWindow="1788" windowWidth="14292" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cortes" sheetId="1" r:id="rId1"/>
+    <sheet name="Cortes" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Nombre Calle</t>
+    <t>Calle Cortada</t>
   </si>
   <si>
     <t>Calle de Ayala</t>
@@ -46,13 +46,13 @@
     <t>Calle de San Patricio</t>
   </si>
   <si>
-    <t>Avda  Complutense</t>
+    <t>Avda Complutense</t>
   </si>
   <si>
     <t>Calle de Melchor Fernández Almagro</t>
   </si>
   <si>
-    <t>Cmno  Antiguo Viejo de Vicálvaro</t>
+    <t>Cmno Antiguo Viejo de Vicálvaro</t>
   </si>
 </sst>
 </file>
@@ -400,24 +400,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="200.7265625" customWidth="1"/>
-    <col min="2" max="2" width="3.7265625" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="7" width="6.7265625" customWidth="1"/>
-    <col min="8" max="8" width="51.7265625" customWidth="1"/>
-    <col min="9" max="10" width="100.7265625" customWidth="1"/>
-    <col min="11" max="11" width="5.7265625" customWidth="1"/>
+    <col min="1" max="1" width="37.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -481,11 +473,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DDB66BF3C975CA4CBC680BCE2F760A29" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80f7db915f4810ea9277f6a39fcd2a37">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d4832a78-f68e-4d9f-b9e0-99267fa86e76" xmlns:ns3="3980694b-12ad-4614-af6b-880c0e4c72ba" xmlns:ns4="a232ef0a-c86e-4657-a615-844f9bf8468b" xmlns:ns5="aaefd727-9cb6-4c02-9ace-b3a3b4c9f10e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33f5fe8646a8ab7c81e4c914f27ad887" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
-    <xsd:import namespace="d4832a78-f68e-4d9f-b9e0-99267fa86e76"/>
-    <xsd:import namespace="3980694b-12ad-4614-af6b-880c0e4c72ba"/>
-    <xsd:import namespace="a232ef0a-c86e-4657-a615-844f9bf8468b"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="01c41473-b863-49d2-b0dd-3ca8cb10dade">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="aaefd727-9cb6-4c02-9ace-b3a3b4c9f10e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001D730DDADBE1A042A914DC2F5130D599" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="8b23664a4cac8ea7c25950aa13059c9d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01c41473-b863-49d2-b0dd-3ca8cb10dade" xmlns:ns3="f8dbf3a9-e269-4c96-b391-e46e21159a99" xmlns:ns4="aaefd727-9cb6-4c02-9ace-b3a3b4c9f10e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2da9b021f92415ea3cbfda4239b59774" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="01c41473-b863-49d2-b0dd-3ca8cb10dade"/>
+    <xsd:import namespace="f8dbf3a9-e269-4c96-b391-e46e21159a99"/>
     <xsd:import namespace="aaefd727-9cb6-4c02-9ace-b3a3b4c9f10e"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -495,21 +497,21 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns4:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns5:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns4:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -517,7 +519,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d4832a78-f68e-4d9f-b9e0-99267fa86e76" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="01c41473-b863-49d2-b0dd-3ca8cb10dade" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -530,11 +532,77 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="acecb2a3-f75d-49a1-aafb-d28fcb05aaf5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3980694b-12ad-4614-af6b-880c0e4c72ba" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f8dbf3a9-e269-4c96-b391-e46e21159a99" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -553,88 +621,18 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a232ef0a-c86e-4657-a615-844f9bf8468b" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="acecb2a3-f75d-49a1-aafb-d28fcb05aaf5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="aaefd727-9cb6-4c02-9ace-b3a3b4c9f10e" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{caf3ae2c-12dc-4e46-8801-adf0a65b102e}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="3980694b-12ad-4614-af6b-880c0e4c72ba">
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{fa265715-972c-4e0b-871c-2d03b32f34e3}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="f8dbf3a9-e269-4c96-b391-e46e21159a99">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -745,7 +743,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -755,9 +753,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E141A36-7908-454E-9599-7374C69260BB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F52E947D-86AC-44BD-9458-7E9794865BC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="01c41473-b863-49d2-b0dd-3ca8cb10dade"/>
+    <ds:schemaRef ds:uri="aaefd727-9cb6-4c02-9ace-b3a3b4c9f10e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7239480-57A4-4FBB-B949-1C04302868DA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D41A10D-09DE-4AC1-81F5-E64D999D4F67}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB853863-E941-4B9A-97F3-590D104D9AC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>